<commit_message>
More fixes requested by client.
</commit_message>
<xml_diff>
--- a/dashboard_loader/health_smoking_uploader/health_smoking.xlsx
+++ b/dashboard_loader/health_smoking_uploader/health_smoking.xlsx
@@ -101,7 +101,7 @@
     <t xml:space="preserve">Desc Body</t>
   </si>
   <si>
-    <t xml:space="preserve">In 2014-15, 14.8 per cent of Australian adults were daily smokers. Nationally, between 2007-08 and 2014-15 there was a significant fall in the rate of smoking (4.3 percentage points), and significant falls in all states and territories except for the Northern Territory</t>
+    <t xml:space="preserve">In 2014-15, 14.8 per cent of Australian adults were daily smokers. Nationally, between 2007-08 and 2014-15 there was a significant fall in the rate of smoking (4.3 percentage points), and significant falls in all states and territories except for the Northern Territory.</t>
   </si>
   <si>
     <t xml:space="preserve">While smoking rates have fallen over time, they will need to fall faster to meet the benchmark set by COAG.</t>
@@ -126,7 +126,7 @@
     <t xml:space="preserve">ABS (unpublished) National Health Survey 2014-15</t>
   </si>
   <si>
-    <t xml:space="preserve">ABS (unpublished) Australian Health Survey 2011­13 (2011­12 core component)</t>
+    <t xml:space="preserve">ABS (unpublished) Australian Health Survey 2011­-13 (2011-­12 core component)</t>
   </si>
   <si>
     <t xml:space="preserve">ABS (unpublished) National Health Survey 2007-08.</t>
@@ -142,7 +142,7 @@
     <numFmt numFmtId="166" formatCode="########\ ###\ ##0.0;\-########\ ###\ ##0.0;\–"/>
     <numFmt numFmtId="167" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -163,87 +163,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -267,7 +186,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,74 +195,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -361,7 +223,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -385,55 +247,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -443,39 +257,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="2" xfId="36" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="36" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="3" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -484,91 +298,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="36" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -580,7 +318,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B8:B13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -993,12 +731,12 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8:B13"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="85.17"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
@@ -1035,7 +773,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>